<commit_message>
update vals with new BTT BCT grid
</commit_message>
<xml_diff>
--- a/scint_plots/peak_flux_performance/peak_dt.xlsx
+++ b/scint_plots/peak_flux_performance/peak_dt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\scint_plots\scint_plots\peak_flux_performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02306819-E866-465F-9130-D0BF3C2A6C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B365180-9F90-4A03-80AA-41FDEB35458A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1350" windowWidth="29040" windowHeight="15840" xr2:uid="{12FF4ADC-7C1A-4B40-B735-649D4F96C037}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{12FF4ADC-7C1A-4B40-B735-649D4F96C037}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -425,8 +425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B13A79D4-36A9-4E27-B988-DF63CC0DA7EF}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +497,7 @@
         <v>27</v>
       </c>
       <c r="D4">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E4">
         <v>12</v>
@@ -531,7 +531,7 @@
         <v>25</v>
       </c>
       <c r="D6">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6">
         <v>5</v>
@@ -548,7 +548,7 @@
         <v>16</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -565,7 +565,7 @@
         <v>2</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -648,7 +648,7 @@
       </c>
       <c r="D12">
         <f t="shared" si="3"/>
-        <v>31.578947368421051</v>
+        <v>36.84210526315789</v>
       </c>
       <c r="E12">
         <f t="shared" si="4"/>
@@ -690,7 +690,7 @@
       </c>
       <c r="D14">
         <f t="shared" si="3"/>
-        <v>21.052631578947366</v>
+        <v>19.298245614035086</v>
       </c>
       <c r="E14">
         <f t="shared" si="4"/>
@@ -711,7 +711,7 @@
       </c>
       <c r="D15">
         <f t="shared" si="3"/>
-        <v>8.7719298245614024</v>
+        <v>7.0175438596491224</v>
       </c>
       <c r="E15">
         <f t="shared" si="4"/>
@@ -732,7 +732,7 @@
       </c>
       <c r="D16">
         <f t="shared" si="3"/>
-        <v>7.0175438596491224</v>
+        <v>5.2631578947368416</v>
       </c>
       <c r="E16">
         <f t="shared" si="4"/>

</xml_diff>